<commit_message>
add another feature file
</commit_message>
<xml_diff>
--- a/src/test/TestData/MainDataSheet.xlsx
+++ b/src/test/TestData/MainDataSheet.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC_01" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="TC_02" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -131,6 +132,123 @@
   </si>
   <si>
     <t xml:space="preserve">The form was successfully submitted!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txt_search_box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@id='search_query_top']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[@name='submit_search']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_product_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//img[@title='Printed Chiffon Dress']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icon_plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//i[@class='icon-plus']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//select[@id='group_1']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//a[@id='color_15']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//span[contains(text(),'Add to cart')]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_proceed_to_checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//a[@title='Proceed to checkout']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txt_email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@id='email']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18naduni@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txt_password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//input[@id='passwd']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hnUg2kaF@MaUrfr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[@id='SubmitLogin']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//a[@href='http://automationpractice.com/index.php?controller=order&amp;step=1']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_checkout2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[@name='processAddress']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chk_agree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//div[@id='uniform-cgv']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_checkout3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//button[@name='processCarrier']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_shipping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//a[@title='Pay by bank wire']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn_confirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//span[text()='I confirm my order']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txt_confirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//strong[text()='Your order will be sent as soon as we receive payment.']</t>
   </si>
 </sst>
 </file>
@@ -141,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,6 +280,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,7 +329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,6 +339,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,11 +365,11 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.06"/>
@@ -402,4 +529,200 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.12"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug in screenshot capturing and edit gitignore
</commit_message>
<xml_diff>
--- a/src/test/TestData/MainDataSheet.xlsx
+++ b/src/test/TestData/MainDataSheet.xlsx
@@ -167,7 +167,7 @@
     <t xml:space="preserve">//select[@id='group_1']</t>
   </si>
   <si>
-    <t xml:space="preserve">M</t>
+    <t xml:space="preserve">Ms</t>
   </si>
   <si>
     <t xml:space="preserve">btn_color</t>
@@ -259,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -280,11 +280,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -329,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,10 +334,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,7 +360,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.06"/>
@@ -539,10 +530,10 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.3"/>
@@ -664,7 +655,7 @@
       <c r="A13" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>